<commit_message>
Added advertisment Display all and single, Added archive, view functionality
</commit_message>
<xml_diff>
--- a/classyad.xlsx
+++ b/classyad.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t>user</t>
   </si>
@@ -348,27 +348,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -380,19 +386,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,7 +679,7 @@
   <dimension ref="B1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="L5" sqref="L5:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
       <c r="E2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="31"/>
+      <c r="G2" s="15"/>
       <c r="H2" s="1" t="s">
         <v>55</v>
       </c>
@@ -721,43 +721,43 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="J5" s="22" t="s">
+      <c r="J5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22" t="s">
+      <c r="K5" s="17"/>
+      <c r="L5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22" t="s">
+      <c r="M5" s="17"/>
+      <c r="N5" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
       <c r="H6" s="4"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
@@ -778,39 +778,39 @@
       <c r="N7" s="21"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="27" t="s">
+      <c r="D8" s="23"/>
+      <c r="E8" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="25"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="3"/>
       <c r="I8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17" t="s">
+      <c r="K8" s="16"/>
+      <c r="L8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="17"/>
+      <c r="M8" s="16"/>
       <c r="N8" s="8"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="25"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="3"/>
       <c r="I9" s="11"/>
       <c r="J9" s="21" t="s">
@@ -822,62 +822,62 @@
       <c r="N9" s="21"/>
     </row>
     <row r="10" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" s="28" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="27" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="25"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
       <c r="N10" s="8"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="25"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="17" t="s">
+      <c r="I11" s="25"/>
+      <c r="J11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
       <c r="N11" s="8"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="6"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="17" t="s">
+      <c r="I12" s="25"/>
+      <c r="J12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
       <c r="N12" s="8"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
@@ -890,29 +890,29 @@
       <c r="F13" s="19"/>
       <c r="G13" s="20"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="17" t="s">
+      <c r="I13" s="26"/>
+      <c r="J13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17" t="s">
+      <c r="K13" s="16"/>
+      <c r="L13" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="17"/>
+      <c r="M13" s="16"/>
       <c r="N13" s="8"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17" t="s">
+      <c r="D14" s="16"/>
+      <c r="E14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="17"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="7"/>
       <c r="H14" s="3"/>
       <c r="I14" s="11"/>
@@ -925,36 +925,36 @@
       <c r="N14" s="21"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-      <c r="C15" s="17" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="8"/>
       <c r="H15" s="3"/>
       <c r="I15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17" t="s">
+      <c r="K15" s="16"/>
+      <c r="L15" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="17"/>
+      <c r="M15" s="16"/>
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="8"/>
       <c r="H16" s="3"/>
       <c r="I16" s="11"/>
@@ -976,80 +976,80 @@
       <c r="F17" s="19"/>
       <c r="G17" s="20"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17" t="s">
+      <c r="K17" s="16"/>
+      <c r="L17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="M17" s="17"/>
+      <c r="M17" s="16"/>
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="8"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="17" t="s">
+      <c r="I18" s="28"/>
+      <c r="J18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17" t="s">
+      <c r="K18" s="16"/>
+      <c r="L18" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="M18" s="17"/>
+      <c r="M18" s="16"/>
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
       <c r="G19" s="8"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="17" t="s">
+      <c r="I19" s="28"/>
+      <c r="J19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
       <c r="N19" s="8"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="22"/>
+      <c r="C20" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
       <c r="G20" s="8"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="17" t="s">
+      <c r="I20" s="28"/>
+      <c r="J20" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17" t="s">
+      <c r="K20" s="16"/>
+      <c r="L20" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="17"/>
+      <c r="M20" s="16"/>
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
@@ -1075,24 +1075,26 @@
       <c r="B22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
       <c r="G22" s="8"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="J22" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="8"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="16"/>
+      <c r="N22" s="7"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
@@ -1104,27 +1106,29 @@
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17" t="s">
+      <c r="I23" s="29"/>
+      <c r="J23" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="8"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M23" s="16"/>
+      <c r="N23" s="7"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17" t="s">
+      <c r="D24" s="16"/>
+      <c r="E24" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="17"/>
+      <c r="F24" s="16"/>
       <c r="G24" s="7"/>
       <c r="I24" s="9"/>
       <c r="J24" s="18" t="s">
@@ -1136,23 +1140,23 @@
       <c r="N24" s="20"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="16"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="8"/>
       <c r="I25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J25" s="17" t="s">
+      <c r="J25" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17" t="s">
+      <c r="K25" s="16"/>
+      <c r="L25" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M25" s="17"/>
+      <c r="M25" s="16"/>
       <c r="N25" s="7"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
@@ -1166,51 +1170,63 @@
       <c r="N26" s="21"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I27" s="15" t="s">
+      <c r="I27" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="17" t="s">
+      <c r="J27" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
       <c r="N27" s="8"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I28" s="16"/>
-      <c r="J28" s="17" t="s">
+      <c r="I28" s="29"/>
+      <c r="J28" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
       <c r="N28" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="L5:M6"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="J16:N16"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="I17:I20"/>
+    <mergeCell ref="C13:G13"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="C8:D9"/>
@@ -1227,50 +1243,38 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="L5:M6"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L23:M23"/>
     <mergeCell ref="E8:F9"/>
     <mergeCell ref="E10:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="C23:G23"/>
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="J7:N7"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="J16:N16"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="I10:I13"/>
     <mergeCell ref="C7:G7"/>
-    <mergeCell ref="G8:G9"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="I17:I20"/>
-    <mergeCell ref="C13:G13"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="C21:G21"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -1319,33 +1323,33 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="J5" s="17" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
@@ -1364,15 +1368,15 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31"/>
       <c r="G8" s="9"/>
       <c r="I8" s="14" t="s">
         <v>44</v>
@@ -1382,13 +1386,13 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
-      <c r="C9" s="29" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="9"/>
       <c r="I9" s="14" t="s">
         <v>10</v>
@@ -1398,13 +1402,13 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" s="29" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="30"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="9"/>
       <c r="I10" s="14" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Added image upload, Added water mark to the images,Added indiviual view of the advertisement
</commit_message>
<xml_diff>
--- a/classyad.xlsx
+++ b/classyad.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Classy Ad" sheetId="1" r:id="rId1"/>
-    <sheet name="SHRM" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="SHRM" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>user</t>
   </si>
@@ -189,6 +190,12 @@
   </si>
   <si>
     <t>Requires Server For mail notification, and identity verfication</t>
+  </si>
+  <si>
+    <t>completed by adding archive</t>
+  </si>
+  <si>
+    <t>watermark</t>
   </si>
 </sst>
 </file>
@@ -352,41 +359,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -678,8 +685,8 @@
   </sheetPr>
   <dimension ref="B1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:M6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,75 +728,75 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17" t="s">
+      <c r="D5" s="28"/>
+      <c r="E5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17" t="s">
+      <c r="F5" s="28"/>
+      <c r="G5" s="28" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17" t="s">
+      <c r="K5" s="28"/>
+      <c r="L5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17" t="s">
+      <c r="M5" s="28"/>
+      <c r="N5" s="28" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="4"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="3"/>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="29" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="16"/>
-      <c r="G8" s="27"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="3"/>
       <c r="I8" s="10" t="s">
         <v>1</v>
@@ -805,35 +812,35 @@
       <c r="N8" s="8"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="27"/>
+      <c r="G9" s="22"/>
       <c r="H9" s="3"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24" t="s">
+      <c r="D10" s="27"/>
+      <c r="E10" s="29" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="16"/>
-      <c r="G10" s="27"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="20" t="s">
         <v>27</v>
       </c>
       <c r="J10" s="16" t="s">
@@ -845,24 +852,26 @@
       <c r="N10" s="8"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="27"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="25"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="16" t="s">
         <v>7</v>
       </c>
       <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
+      <c r="L11" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="M11" s="16"/>
-      <c r="N11" s="8"/>
+      <c r="N11" s="7"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="16" t="s">
         <v>5</v>
       </c>
@@ -871,26 +880,28 @@
       <c r="F12" s="16"/>
       <c r="G12" s="6"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="25"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="16" t="s">
         <v>8</v>
       </c>
       <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
+      <c r="L12" s="16" t="s">
+        <v>56</v>
+      </c>
       <c r="M12" s="16"/>
-      <c r="N12" s="8"/>
+      <c r="N12" s="7"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="26"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="26"/>
+      <c r="I13" s="21"/>
       <c r="J13" s="16" t="s">
         <v>29</v>
       </c>
@@ -902,7 +913,7 @@
       <c r="N13" s="8"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -916,16 +927,16 @@
       <c r="G14" s="7"/>
       <c r="H14" s="3"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="16" t="s">
         <v>7</v>
       </c>
@@ -948,7 +959,7 @@
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="16" t="s">
         <v>8</v>
       </c>
@@ -958,25 +969,25 @@
       <c r="G16" s="8"/>
       <c r="H16" s="3"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J17" s="16" t="s">
@@ -990,7 +1001,7 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="16" t="s">
@@ -1001,7 +1012,7 @@
       <c r="F18" s="16"/>
       <c r="G18" s="8"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="28"/>
+      <c r="I18" s="23"/>
       <c r="J18" s="16" t="s">
         <v>6</v>
       </c>
@@ -1013,7 +1024,7 @@
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="16" t="s">
         <v>13</v>
       </c>
@@ -1022,7 +1033,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="8"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="28"/>
+      <c r="I19" s="23"/>
       <c r="J19" s="16" t="s">
         <v>7</v>
       </c>
@@ -1032,7 +1043,7 @@
       <c r="N19" s="8"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="16" t="s">
         <v>14</v>
       </c>
@@ -1041,7 +1052,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="8"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="28"/>
+      <c r="I20" s="23"/>
       <c r="J20" s="16" t="s">
         <v>8</v>
       </c>
@@ -1054,22 +1065,22 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
       <c r="H21" s="3"/>
       <c r="I21" s="11"/>
-      <c r="J21" s="21" t="s">
+      <c r="J21" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
@@ -1083,7 +1094,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="8"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="22" t="s">
+      <c r="I22" s="17" t="s">
         <v>21</v>
       </c>
       <c r="J22" s="16" t="s">
@@ -1098,15 +1109,15 @@
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="29"/>
+      <c r="I23" s="18"/>
       <c r="J23" s="16" t="s">
         <v>23</v>
       </c>
@@ -1118,7 +1129,7 @@
       <c r="N23" s="7"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="17" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="16" t="s">
@@ -1131,16 +1142,16 @@
       <c r="F24" s="16"/>
       <c r="G24" s="7"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="18" t="s">
+      <c r="J24" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="20"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="26"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="29"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1161,16 +1172,16 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I26" s="11"/>
-      <c r="J26" s="21" t="s">
+      <c r="J26" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="17" t="s">
         <v>36</v>
       </c>
       <c r="J27" s="16" t="s">
@@ -1182,7 +1193,7 @@
       <c r="N27" s="8"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I28" s="29"/>
+      <c r="I28" s="18"/>
       <c r="J28" s="16" t="s">
         <v>7</v>
       </c>
@@ -1193,24 +1204,48 @@
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="L5:M6"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="E10:F11"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="C12:D12"/>
@@ -1227,54 +1262,30 @@
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="I17:I20"/>
     <mergeCell ref="C13:G13"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
     <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="L5:M6"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="E8:F9"/>
-    <mergeCell ref="E10:F11"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -1283,13 +1294,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,43 +1357,43 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17" t="s">
+      <c r="D5" s="28"/>
+      <c r="E5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17" t="s">
+      <c r="F5" s="28"/>
+      <c r="G5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="28" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
       <c r="I7" s="14" t="s">
         <v>43</v>
       </c>
@@ -1368,7 +1402,7 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="17" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="30" t="s">
@@ -1386,7 +1420,7 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="30" t="s">
         <v>52</v>
       </c>
@@ -1402,7 +1436,7 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="30" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Added Membership Plans View Edit Add Delete In admin panel, Resized the image and added watermark
</commit_message>
<xml_diff>
--- a/classyad.xlsx
+++ b/classyad.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>user</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>watermark</t>
+  </si>
+  <si>
+    <t>Session Problem</t>
+  </si>
+  <si>
+    <t>Search Functionality</t>
+  </si>
+  <si>
+    <t>Location Tracking</t>
+  </si>
+  <si>
+    <t>Transaction</t>
   </si>
 </sst>
 </file>
@@ -258,7 +270,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -355,17 +367,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -376,30 +401,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,10 +711,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="B1:N28"/>
+  <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +743,7 @@
       <c r="E2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="15"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="1" t="s">
         <v>55</v>
       </c>
@@ -728,482 +756,573 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28" t="s">
+      <c r="D5" s="16"/>
+      <c r="E5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="16" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28" t="s">
+      <c r="K5" s="16"/>
+      <c r="L5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28" t="s">
+      <c r="M5" s="16"/>
+      <c r="N5" s="16" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="4"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="3"/>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="29" t="s">
+      <c r="D8" s="30"/>
+      <c r="E8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="22"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="3"/>
       <c r="I8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16" t="s">
+      <c r="K8" s="15"/>
+      <c r="L8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="16"/>
-      <c r="N8" s="8"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="3"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
     </row>
     <row r="10" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
-      <c r="C10" s="27" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="29" t="s">
+      <c r="D10" s="30"/>
+      <c r="E10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="22"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="25"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
       <c r="N10" s="8"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="16" t="s">
+      <c r="I11" s="23"/>
+      <c r="J11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16" t="s">
+      <c r="K11" s="15"/>
+      <c r="L11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="16"/>
+      <c r="M11" s="15"/>
       <c r="N11" s="7"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="16" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="6"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="16" t="s">
+      <c r="I12" s="23"/>
+      <c r="J12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16" t="s">
+      <c r="K12" s="15"/>
+      <c r="L12" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="M12" s="16"/>
+      <c r="M12" s="15"/>
       <c r="N12" s="7"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="16" t="s">
+      <c r="I13" s="24"/>
+      <c r="J13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16" t="s">
+      <c r="K13" s="15"/>
+      <c r="L13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="16"/>
-      <c r="N13" s="8"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="7"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16" t="s">
+      <c r="D14" s="31"/>
+      <c r="E14" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="16"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="7"/>
       <c r="H14" s="3"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="16" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="8"/>
       <c r="H15" s="3"/>
       <c r="I15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="J15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16" t="s">
+      <c r="K15" s="15"/>
+      <c r="L15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="16"/>
+      <c r="M15" s="15"/>
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
-      <c r="C16" s="16" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="8"/>
       <c r="H16" s="3"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="J17" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16" t="s">
+      <c r="K17" s="15"/>
+      <c r="L17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="M17" s="16"/>
+      <c r="M17" s="15"/>
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="8"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="16" t="s">
+      <c r="I18" s="26"/>
+      <c r="J18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16" t="s">
+      <c r="K18" s="15"/>
+      <c r="L18" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="M18" s="16"/>
+      <c r="M18" s="15"/>
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="8"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="16" t="s">
+      <c r="I19" s="26"/>
+      <c r="J19" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
       <c r="N19" s="8"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="17"/>
-      <c r="C20" s="16" t="s">
+      <c r="B20" s="22"/>
+      <c r="C20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="8"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="16" t="s">
+      <c r="I20" s="26"/>
+      <c r="J20" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16" t="s">
+      <c r="K20" s="15"/>
+      <c r="L20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="16"/>
+      <c r="M20" s="15"/>
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19"/>
       <c r="H21" s="3"/>
       <c r="I21" s="11"/>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
       <c r="G22" s="8"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="16" t="s">
+      <c r="J22" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16" t="s">
+      <c r="K22" s="15"/>
+      <c r="L22" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M22" s="16"/>
+      <c r="M22" s="15"/>
       <c r="N22" s="7"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="16" t="s">
+      <c r="I23" s="27"/>
+      <c r="J23" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16" t="s">
+      <c r="K23" s="15"/>
+      <c r="L23" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="16"/>
+      <c r="M23" s="15"/>
       <c r="N23" s="7"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16" t="s">
+      <c r="D24" s="15"/>
+      <c r="E24" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="15"/>
       <c r="G24" s="7"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="24" t="s">
+      <c r="J24" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="26"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="19"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
       <c r="G25" s="8"/>
       <c r="I25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J25" s="16" t="s">
+      <c r="J25" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16" t="s">
+      <c r="K25" s="15"/>
+      <c r="L25" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M25" s="16"/>
+      <c r="M25" s="15"/>
       <c r="N25" s="7"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I26" s="11"/>
-      <c r="J26" s="19" t="s">
+      <c r="J26" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="16" t="s">
+      <c r="J27" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="8"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M27" s="15"/>
+      <c r="N27" s="7"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I28" s="18"/>
-      <c r="J28" s="16" t="s">
+      <c r="I28" s="27"/>
+      <c r="J28" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="8"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" s="15"/>
+      <c r="N28" s="7"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J29" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="36"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I30" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="J30" s="38"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="82">
+  <mergeCells count="84">
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="J16:N16"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="I17:I20"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J11:K11"/>
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="C5:D6"/>
@@ -1220,72 +1339,6 @@
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="C17:G17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="J16:N16"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="I10:I13"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="I17:I20"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="J17:K17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -1294,20 +1347,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4"/>
+  <dimension ref="C4:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="C4" s="33" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1323,7 +1391,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E8" sqref="E8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,43 +1425,43 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28" t="s">
+      <c r="D5" s="16"/>
+      <c r="E5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="16" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
       <c r="I7" s="14" t="s">
         <v>43</v>
       </c>
@@ -1402,15 +1470,15 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="9"/>
       <c r="I8" s="14" t="s">
         <v>44</v>
@@ -1420,13 +1488,13 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
-      <c r="C9" s="30" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="9"/>
       <c r="I9" s="14" t="s">
         <v>10</v>
@@ -1436,13 +1504,13 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
-      <c r="C10" s="30" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="9"/>
       <c r="I10" s="14" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Added succesful payment gateway sample, Not adding the payment status in the db
</commit_message>
<xml_diff>
--- a/classyad.xlsx
+++ b/classyad.xlsx
@@ -372,6 +372,47 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -386,47 +427,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,8 +713,8 @@
   </sheetPr>
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17:I20"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,492 +756,492 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38" t="s">
+      <c r="F5" s="21"/>
+      <c r="G5" s="21" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38" t="s">
+      <c r="K5" s="21"/>
+      <c r="L5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38" t="s">
+      <c r="M5" s="21"/>
+      <c r="N5" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
       <c r="H6" s="4"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="3"/>
-      <c r="J7" s="29" t="s">
+      <c r="J7" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="39" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="35"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="32"/>
       <c r="H8" s="3"/>
       <c r="I8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26" t="s">
+      <c r="K8" s="20"/>
+      <c r="L8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="26"/>
+      <c r="M8" s="20"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="35"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="32"/>
       <c r="H9" s="3"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
     </row>
     <row r="10" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="27"/>
-      <c r="C10" s="37" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="39" t="s">
+      <c r="D10" s="27"/>
+      <c r="E10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="35"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="32"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="33" t="s">
+      <c r="I10" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
       <c r="N10" s="8"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="27"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="35"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="32"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="26" t="s">
+      <c r="I11" s="30"/>
+      <c r="J11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26" t="s">
+      <c r="K11" s="20"/>
+      <c r="L11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="26"/>
+      <c r="M11" s="20"/>
       <c r="N11" s="7"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="27"/>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="28"/>
+      <c r="C12" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="6"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="26" t="s">
+      <c r="I12" s="30"/>
+      <c r="J12" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26" t="s">
+      <c r="K12" s="20"/>
+      <c r="L12" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="M12" s="26"/>
+      <c r="M12" s="20"/>
       <c r="N12" s="7"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="32"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="26" t="s">
+      <c r="I13" s="31"/>
+      <c r="J13" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26" t="s">
+      <c r="K13" s="20"/>
+      <c r="L13" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="26"/>
+      <c r="M13" s="20"/>
       <c r="N13" s="7"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="26"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="7"/>
       <c r="H14" s="3"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
-      <c r="C15" s="25" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="8"/>
       <c r="H15" s="3"/>
       <c r="I15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26" t="s">
+      <c r="K15" s="20"/>
+      <c r="L15" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="26"/>
+      <c r="M15" s="20"/>
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="27"/>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="28"/>
+      <c r="C16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="8"/>
       <c r="H16" s="3"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="32"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="27" t="s">
+      <c r="I17" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26" t="s">
+      <c r="K17" s="20"/>
+      <c r="L17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M17" s="26"/>
+      <c r="M17" s="20"/>
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="8"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="26" t="s">
+      <c r="I18" s="33"/>
+      <c r="J18" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26" t="s">
+      <c r="K18" s="20"/>
+      <c r="L18" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M18" s="26"/>
+      <c r="M18" s="20"/>
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="27"/>
-      <c r="C19" s="26" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="8"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="26" t="s">
+      <c r="I19" s="33"/>
+      <c r="J19" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
       <c r="N19" s="8"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
-      <c r="C20" s="26" t="s">
+      <c r="B20" s="28"/>
+      <c r="C20" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
       <c r="G20" s="8"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="26" t="s">
+      <c r="I20" s="33"/>
+      <c r="J20" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26" t="s">
+      <c r="K20" s="20"/>
+      <c r="L20" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="26"/>
+      <c r="M20" s="20"/>
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="32"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="3"/>
       <c r="I21" s="11"/>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="8"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="27" t="s">
+      <c r="I22" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="J22" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26" t="s">
+      <c r="K22" s="20"/>
+      <c r="L22" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M22" s="26"/>
+      <c r="M22" s="20"/>
       <c r="N22" s="7"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="26" t="s">
+      <c r="I23" s="34"/>
+      <c r="J23" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26" t="s">
+      <c r="K23" s="20"/>
+      <c r="L23" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="26"/>
+      <c r="M23" s="20"/>
       <c r="N23" s="7"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26" t="s">
+      <c r="D24" s="20"/>
+      <c r="E24" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="26"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="7"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="30" t="s">
+      <c r="J24" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="32"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="24"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="28"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="8"/>
       <c r="I25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J25" s="26" t="s">
+      <c r="J25" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26" t="s">
+      <c r="K25" s="20"/>
+      <c r="L25" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M25" s="26"/>
+      <c r="M25" s="20"/>
       <c r="N25" s="7"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I26" s="11"/>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I27" s="27" t="s">
+      <c r="I27" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="26" t="s">
+      <c r="J27" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26" t="s">
+      <c r="K27" s="20"/>
+      <c r="L27" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="M27" s="26"/>
+      <c r="M27" s="20"/>
       <c r="N27" s="7"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I28" s="28"/>
-      <c r="J28" s="26" t="s">
+      <c r="I28" s="34"/>
+      <c r="J28" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26" t="s">
+      <c r="K28" s="20"/>
+      <c r="L28" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M28" s="26"/>
+      <c r="M28" s="20"/>
       <c r="N28" s="7"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J29" s="20" t="s">
+      <c r="J29" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="22"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="37"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I30" s="17" t="s">
@@ -1249,12 +1249,80 @@
       </c>
       <c r="J30" s="18"/>
       <c r="K30" s="19"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="24"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="39"/>
       <c r="N30" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="J16:N16"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="I17:I20"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="L25:M25"/>
@@ -1271,74 +1339,6 @@
     <mergeCell ref="J7:N7"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="J16:N16"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="I10:I13"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="I17:I20"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -1425,43 +1425,43 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38" t="s">
+      <c r="F5" s="21"/>
+      <c r="G5" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="21" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
       <c r="I7" s="14" t="s">
         <v>43</v>
       </c>
@@ -1470,15 +1470,15 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="9"/>
       <c r="I8" s="14" t="s">
         <v>44</v>
@@ -1488,13 +1488,13 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="9"/>
       <c r="I9" s="14" t="s">
         <v>10</v>
@@ -1504,13 +1504,13 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="27"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="9"/>
       <c r="I10" s="14" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Added Dashboard widgets in admin panel
</commit_message>
<xml_diff>
--- a/classyad.xlsx
+++ b/classyad.xlsx
@@ -339,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -370,63 +370,61 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,8 +711,8 @@
   </sheetPr>
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,520 +754,558 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21" t="s">
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="36"/>
+      <c r="G5" s="36" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21" t="s">
+      <c r="K5" s="36"/>
+      <c r="L5" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21" t="s">
+      <c r="M5" s="36"/>
+      <c r="N5" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="4"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="3"/>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="25" t="s">
+      <c r="D8" s="35"/>
+      <c r="E8" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="32"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="33"/>
       <c r="H8" s="3"/>
       <c r="I8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20" t="s">
+      <c r="K8" s="24"/>
+      <c r="L8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="20"/>
+      <c r="M8" s="24"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="32"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="3"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
     </row>
     <row r="10" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
-      <c r="C10" s="27" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="25" t="s">
+      <c r="D10" s="35"/>
+      <c r="E10" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="32"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
       <c r="N10" s="8"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="32"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="20" t="s">
+      <c r="I11" s="31"/>
+      <c r="J11" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20" t="s">
+      <c r="K11" s="24"/>
+      <c r="L11" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="20"/>
+      <c r="M11" s="24"/>
       <c r="N11" s="7"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
-      <c r="C12" s="29" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="6"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="20" t="s">
+      <c r="I12" s="31"/>
+      <c r="J12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20" t="s">
+      <c r="K12" s="24"/>
+      <c r="L12" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="M12" s="20"/>
+      <c r="M12" s="24"/>
       <c r="N12" s="7"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="24"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="30"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="20" t="s">
+      <c r="I13" s="32"/>
+      <c r="J13" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20" t="s">
+      <c r="K13" s="24"/>
+      <c r="L13" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="20"/>
+      <c r="M13" s="24"/>
       <c r="N13" s="7"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="20" t="s">
+      <c r="D14" s="23"/>
+      <c r="E14" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="20"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="7"/>
       <c r="H14" s="3"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="C15" s="29" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="8"/>
       <c r="H15" s="3"/>
       <c r="I15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20" t="s">
+      <c r="K15" s="24"/>
+      <c r="L15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="20"/>
+      <c r="M15" s="24"/>
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
-      <c r="C16" s="29" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="8"/>
       <c r="H16" s="3"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20" t="s">
+      <c r="K17" s="24"/>
+      <c r="L17" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="M17" s="20"/>
+      <c r="M17" s="24"/>
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="8"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="20" t="s">
+      <c r="I18" s="34"/>
+      <c r="J18" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20" t="s">
+      <c r="K18" s="24"/>
+      <c r="L18" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="M18" s="20"/>
+      <c r="M18" s="24"/>
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="28"/>
-      <c r="C19" s="20" t="s">
+      <c r="B19" s="25"/>
+      <c r="C19" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
       <c r="G19" s="8"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="20" t="s">
+      <c r="I19" s="34"/>
+      <c r="J19" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
       <c r="N19" s="8"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="28"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="8"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="20" t="s">
+      <c r="I20" s="34"/>
+      <c r="J20" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20" t="s">
+      <c r="K20" s="24"/>
+      <c r="L20" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="20"/>
+      <c r="M20" s="24"/>
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="30"/>
       <c r="H21" s="3"/>
       <c r="I21" s="11"/>
-      <c r="J21" s="26" t="s">
+      <c r="J21" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
       <c r="G22" s="8"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20" t="s">
+      <c r="K22" s="24"/>
+      <c r="L22" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M22" s="20"/>
+      <c r="M22" s="24"/>
       <c r="N22" s="7"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="20" t="s">
+      <c r="I23" s="26"/>
+      <c r="J23" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20" t="s">
+      <c r="K23" s="24"/>
+      <c r="L23" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="20"/>
+      <c r="M23" s="24"/>
       <c r="N23" s="7"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20" t="s">
+      <c r="D24" s="24"/>
+      <c r="E24" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="20"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="7"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="22" t="s">
+      <c r="J24" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="24"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="30"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="34"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="8"/>
       <c r="I25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J25" s="20" t="s">
+      <c r="J25" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20" t="s">
+      <c r="K25" s="24"/>
+      <c r="L25" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M25" s="20"/>
+      <c r="M25" s="24"/>
       <c r="N25" s="7"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I26" s="11"/>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I27" s="28" t="s">
+      <c r="I27" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="20" t="s">
+      <c r="J27" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20" t="s">
+      <c r="K27" s="24"/>
+      <c r="L27" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="M27" s="20"/>
+      <c r="M27" s="24"/>
       <c r="N27" s="7"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I28" s="34"/>
-      <c r="J28" s="20" t="s">
+      <c r="I28" s="26"/>
+      <c r="J28" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20" t="s">
+      <c r="K28" s="24"/>
+      <c r="L28" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="M28" s="20"/>
+      <c r="M28" s="24"/>
       <c r="N28" s="7"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J29" s="35" t="s">
+      <c r="J29" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="37"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="20"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I30" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J30" s="18"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="9"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="84">
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
+  <mergeCells count="85">
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="L5:M6"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="E10:F11"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="J16:N16"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="I17:I20"/>
+    <mergeCell ref="C13:G13"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="J17:K17"/>
@@ -1286,59 +1322,22 @@
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="C17:G17"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="J16:N16"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="I10:I13"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="I17:I20"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="L5:M6"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="E8:F9"/>
-    <mergeCell ref="E10:F11"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="J30:K30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -1425,43 +1424,43 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21" t="s">
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="36"/>
+      <c r="G5" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="36" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
       <c r="I7" s="14" t="s">
         <v>43</v>
       </c>
@@ -1470,15 +1469,15 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="9"/>
       <c r="I8" s="14" t="s">
         <v>44</v>
@@ -1488,13 +1487,13 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
-      <c r="C9" s="38" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
       <c r="G9" s="9"/>
       <c r="I9" s="14" t="s">
         <v>10</v>
@@ -1504,13 +1503,13 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
-      <c r="C10" s="38" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="9"/>
       <c r="I10" s="14" t="s">
         <v>45</v>

</xml_diff>